<commit_message>
Can generate different cutoff table towards different postive range
</commit_message>
<xml_diff>
--- a/ChangeAnalysis/output/final-cutoff.xlsx
+++ b/ChangeAnalysis/output/final-cutoff.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="21048" windowHeight="9840" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="21045" windowHeight="9840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="final-cutoff" sheetId="1" r:id="rId1"/>
     <sheet name="cutoff-predict" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="tags" sheetId="3" r:id="rId3"/>
+    <sheet name="0.4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="81">
   <si>
     <t>id</t>
   </si>
@@ -246,12 +247,36 @@
     <t>precision</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>model</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cutoff</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>precision</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>recall</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>positive</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>f-measure</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -855,7 +880,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -882,6 +907,12 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -930,17 +961,34 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1161,6 +1209,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1382,6 +1431,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1603,43 +1653,62 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="89676800"/>
-        <c:axId val="89682688"/>
+        <c:smooth val="0"/>
+        <c:axId val="206059392"/>
+        <c:axId val="206060928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89676800"/>
+        <c:axId val="206059392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89682688"/>
+        <c:crossAx val="206060928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89682688"/>
+        <c:axId val="206060928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89676800"/>
+        <c:crossAx val="206059392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1651,12 +1720,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1877,6 +1958,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2098,6 +2180,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2319,34 +2402,51 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="42345600"/>
-        <c:axId val="42347136"/>
+        <c:smooth val="0"/>
+        <c:axId val="205923840"/>
+        <c:axId val="205925376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42345600"/>
+        <c:axId val="205923840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42347136"/>
+        <c:crossAx val="205925376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42347136"/>
+        <c:axId val="205925376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42345600"/>
+        <c:crossAx val="205923840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2354,8 +2454,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2436,7 +2539,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2510,6 +2613,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2544,6 +2648,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2719,33 +2824,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="10.5546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.77734375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="8.875" style="1"/>
+    <col min="10" max="10" width="10.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.75" style="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="1"/>
+    <col min="16" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2786,7 +2891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2827,7 +2932,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2868,7 +2973,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2909,7 +3014,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2950,7 +3055,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2991,7 +3096,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3032,7 +3137,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3073,7 +3178,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3114,7 +3219,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3155,7 +3260,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3196,7 +3301,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3237,7 +3342,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3278,7 +3383,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3319,7 +3424,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3360,7 +3465,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3401,7 +3506,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3442,7 +3547,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3483,7 +3588,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3524,7 +3629,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3565,7 +3670,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3606,7 +3711,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3647,7 +3752,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3688,7 +3793,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3729,7 +3834,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3770,7 +3875,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3811,7 +3916,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3852,7 +3957,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3893,7 +3998,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3934,7 +4039,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3975,7 +4080,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -4016,7 +4121,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -4057,7 +4162,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -4080,7 +4185,7 @@
         <v>0.58230000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -4103,7 +4208,7 @@
         <v>0.58909999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -4126,7 +4231,7 @@
         <v>0.60389999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -4149,7 +4254,7 @@
         <v>0.61439999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -4172,7 +4277,7 @@
         <v>0.61439999999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -4204,19 +4309,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4236,7 +4341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -4256,7 +4361,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -4276,7 +4381,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -4296,7 +4401,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -4316,7 +4421,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -4336,7 +4441,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -4356,7 +4461,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -4376,7 +4481,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -4396,7 +4501,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -4416,7 +4521,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -4436,7 +4541,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -4456,7 +4561,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -4476,7 +4581,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -4496,7 +4601,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -4516,7 +4621,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -4536,7 +4641,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -4556,7 +4661,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -4576,7 +4681,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -4596,7 +4701,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -4616,7 +4721,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -4636,7 +4741,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -4656,7 +4761,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -4676,7 +4781,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -4696,7 +4801,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -4716,7 +4821,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -4736,7 +4841,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -4756,7 +4861,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -4776,7 +4881,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -4796,7 +4901,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -4816,7 +4921,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -4836,7 +4941,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -4856,7 +4961,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B33" s="8">
         <f>AVERAGE(B2:B32)</f>
         <v>0.14620322580645156</v>
@@ -4883,179 +4988,179 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -5064,4 +5169,3021 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="AC36" sqref="AC36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A1" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" t="s">
+        <v>76</v>
+      </c>
+      <c r="U2" t="s">
+        <v>77</v>
+      </c>
+      <c r="V2" t="s">
+        <v>78</v>
+      </c>
+      <c r="W2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.21</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.29070000000000001</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.49859999999999999</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.33460000000000001</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0.63280000000000003</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0.32350000000000001</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.42809999999999998</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O3" s="9">
+        <v>0.36620000000000003</v>
+      </c>
+      <c r="P3" s="9">
+        <v>0.4829</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>0.22559999999999999</v>
+      </c>
+      <c r="R3" s="9">
+        <v>0.3075</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="U3" s="9">
+        <v>0.36620000000000003</v>
+      </c>
+      <c r="V3" s="9">
+        <v>0.4829</v>
+      </c>
+      <c r="W3" s="9">
+        <v>0.22559999999999999</v>
+      </c>
+      <c r="X3" s="9">
+        <v>0.3075</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>0.4536</v>
+      </c>
+      <c r="AB3" s="9">
+        <v>0.25380000000000003</v>
+      </c>
+      <c r="AC3" s="9">
+        <v>9.5699999999999993E-2</v>
+      </c>
+      <c r="AD3" s="9">
+        <v>0.13900000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.54720000000000002</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.29139999999999999</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.38030000000000003</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.54720000000000002</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.29139999999999999</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.38030000000000003</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0.54720000000000002</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>0.29139999999999999</v>
+      </c>
+      <c r="R4" s="9">
+        <v>0.38030000000000003</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="9">
+        <v>0.21</v>
+      </c>
+      <c r="U4" s="9">
+        <v>0.37590000000000001</v>
+      </c>
+      <c r="V4" s="9">
+        <v>0.46</v>
+      </c>
+      <c r="W4" s="9">
+        <v>0.22220000000000001</v>
+      </c>
+      <c r="X4" s="9">
+        <v>0.29970000000000002</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>0.23</v>
+      </c>
+      <c r="AA4" s="9">
+        <v>0.4032</v>
+      </c>
+      <c r="AB4" s="9">
+        <v>0.43580000000000002</v>
+      </c>
+      <c r="AC4" s="9">
+        <v>0.1963</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>0.2707</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.27079999999999999</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.66620000000000001</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.35549999999999998</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.46360000000000001</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.27610000000000001</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.621</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.3251</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.42670000000000002</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0.16</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0.29409999999999997</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0.56910000000000005</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>0.27960000000000002</v>
+      </c>
+      <c r="R5" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="U5" s="9">
+        <v>0.32079999999999997</v>
+      </c>
+      <c r="V5" s="9">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="W5" s="9">
+        <v>0.2203</v>
+      </c>
+      <c r="X5" s="9">
+        <v>0.30380000000000001</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="9">
+        <v>0.21</v>
+      </c>
+      <c r="AA5" s="9">
+        <v>0.35470000000000002</v>
+      </c>
+      <c r="AB5" s="9">
+        <v>0.42320000000000002</v>
+      </c>
+      <c r="AC5" s="9">
+        <v>0.1724</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.13</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.22989999999999999</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.3599</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.49819999999999998</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.26479999999999998</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.25059999999999999</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0.36159999999999998</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O6" s="9">
+        <v>0.26479999999999998</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0.25059999999999999</v>
+      </c>
+      <c r="R6" s="9">
+        <v>0.36159999999999998</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="U6" s="9">
+        <v>0.26939999999999997</v>
+      </c>
+      <c r="V6" s="9">
+        <v>0.60840000000000005</v>
+      </c>
+      <c r="W6" s="9">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="X6" s="9">
+        <v>0.33479999999999999</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="9">
+        <v>0.16</v>
+      </c>
+      <c r="AA6" s="9">
+        <v>0.28860000000000002</v>
+      </c>
+      <c r="AB6" s="9">
+        <v>0.56089999999999995</v>
+      </c>
+      <c r="AC6" s="9">
+        <v>0.19869999999999999</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>0.29349999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.2465</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.74519999999999997</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.39219999999999999</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.51390000000000002</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0.13</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.28210000000000002</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.67789999999999995</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0.31169999999999998</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0.42709999999999998</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0.32650000000000001</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0.58379999999999999</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0.2319</v>
+      </c>
+      <c r="R7" s="9">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T7" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U7" s="9">
+        <v>0.32650000000000001</v>
+      </c>
+      <c r="V7" s="9">
+        <v>0.58379999999999999</v>
+      </c>
+      <c r="W7" s="9">
+        <v>0.2319</v>
+      </c>
+      <c r="X7" s="9">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>0.16</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="AB7" s="9">
+        <v>0.52029999999999998</v>
+      </c>
+      <c r="AC7" s="9">
+        <v>0.19020000000000001</v>
+      </c>
+      <c r="AD7" s="9">
+        <v>0.27850000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.19389999999999999</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.77929999999999999</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.39419999999999999</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.52359999999999995</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0.2235</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0.74460000000000004</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0.32669999999999999</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0.45419999999999999</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="O8" s="9">
+        <v>0.2336</v>
+      </c>
+      <c r="P8" s="9">
+        <v>0.70179999999999998</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>0.29470000000000002</v>
+      </c>
+      <c r="R8" s="9">
+        <v>0.41510000000000002</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="T8" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U8" s="9">
+        <v>0.30070000000000002</v>
+      </c>
+      <c r="V8" s="9">
+        <v>0.58320000000000005</v>
+      </c>
+      <c r="W8" s="9">
+        <v>0.19020000000000001</v>
+      </c>
+      <c r="X8" s="9">
+        <v>0.28689999999999999</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>0.30070000000000002</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>0.58320000000000005</v>
+      </c>
+      <c r="AC8" s="9">
+        <v>0.19020000000000001</v>
+      </c>
+      <c r="AD8" s="9">
+        <v>0.28689999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.1731</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.82050000000000001</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.37269999999999998</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0.1913</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0.77880000000000005</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0.32</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0.4536</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="O9" s="9">
+        <v>0.22059999999999999</v>
+      </c>
+      <c r="P9" s="9">
+        <v>0.74419999999999997</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>0.26519999999999999</v>
+      </c>
+      <c r="R9" s="9">
+        <v>0.3911</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="T9" s="9">
+        <v>0.11</v>
+      </c>
+      <c r="U9" s="9">
+        <v>0.22589999999999999</v>
+      </c>
+      <c r="V9" s="9">
+        <v>0.70809999999999995</v>
+      </c>
+      <c r="W9" s="9">
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="X9" s="9">
+        <v>0.36559999999999998</v>
+      </c>
+      <c r="Y9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="AB9" s="9">
+        <v>0.58279999999999998</v>
+      </c>
+      <c r="AC9" s="9">
+        <v>0.154</v>
+      </c>
+      <c r="AD9" s="9">
+        <v>0.2437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.159</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.86870000000000003</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.35809999999999997</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.50719999999999998</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0.82050000000000001</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0.31080000000000002</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0.45090000000000002</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="O10" s="9">
+        <v>0.1913</v>
+      </c>
+      <c r="P10" s="9">
+        <v>0.77880000000000005</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>0.26690000000000003</v>
+      </c>
+      <c r="R10" s="9">
+        <v>0.39760000000000001</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T10" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="U10" s="9">
+        <v>0.2205</v>
+      </c>
+      <c r="V10" s="9">
+        <v>0.74419999999999997</v>
+      </c>
+      <c r="W10" s="9">
+        <v>0.22120000000000001</v>
+      </c>
+      <c r="X10" s="9">
+        <v>0.34110000000000001</v>
+      </c>
+      <c r="Y10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="AA10" s="9">
+        <v>0.23119999999999999</v>
+      </c>
+      <c r="AB10" s="9">
+        <v>0.70130000000000003</v>
+      </c>
+      <c r="AC10" s="9">
+        <v>0.1988</v>
+      </c>
+      <c r="AD10" s="9">
+        <v>0.30969999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.1694</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.73150000000000004</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.46910000000000002</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.1694</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0.73150000000000004</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0.46910000000000002</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0.18690000000000001</v>
+      </c>
+      <c r="P11" s="9">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0.29149999999999998</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0.40820000000000001</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T11" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="U11" s="9">
+        <v>0.20619999999999999</v>
+      </c>
+      <c r="V11" s="9">
+        <v>0.6401</v>
+      </c>
+      <c r="W11" s="9">
+        <v>0.24829999999999999</v>
+      </c>
+      <c r="X11" s="9">
+        <v>0.35780000000000001</v>
+      </c>
+      <c r="Y11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z11" s="9">
+        <v>0.11</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>0.2402</v>
+      </c>
+      <c r="AB11" s="9">
+        <v>0.57620000000000005</v>
+      </c>
+      <c r="AC11" s="9">
+        <v>0.19189999999999999</v>
+      </c>
+      <c r="AD11" s="9">
+        <v>0.28789999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.1618</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.73150000000000004</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.311</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.43640000000000001</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0.1618</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.73150000000000004</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0.311</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0.43640000000000001</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="O12" s="9">
+        <v>0.18010000000000001</v>
+      </c>
+      <c r="P12" s="9">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="R12" s="9">
+        <v>0.37640000000000001</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="T12" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="U12" s="9">
+        <v>0.1986</v>
+      </c>
+      <c r="V12" s="9">
+        <v>0.64019999999999999</v>
+      </c>
+      <c r="W12" s="9">
+        <v>0.22170000000000001</v>
+      </c>
+      <c r="X12" s="9">
+        <v>0.32940000000000003</v>
+      </c>
+      <c r="Y12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>0.22720000000000001</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>0.61</v>
+      </c>
+      <c r="AC12" s="9">
+        <v>0.18459999999999999</v>
+      </c>
+      <c r="AD12" s="9">
+        <v>0.28349999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.13150000000000001</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.81579999999999997</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.37430000000000002</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.5131</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.15970000000000001</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.73150000000000004</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0.27629999999999999</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O13" s="9">
+        <v>0.15970000000000001</v>
+      </c>
+      <c r="P13" s="9">
+        <v>0.73150000000000004</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>0.27629999999999999</v>
+      </c>
+      <c r="R13" s="9">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="T13" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="U13" s="9">
+        <v>0.17780000000000001</v>
+      </c>
+      <c r="V13" s="9">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="W13" s="9">
+        <v>0.2311</v>
+      </c>
+      <c r="X13" s="9">
+        <v>0.34510000000000002</v>
+      </c>
+      <c r="Y13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z13" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="AA13" s="9">
+        <v>0.19689999999999999</v>
+      </c>
+      <c r="AB13" s="9">
+        <v>0.64019999999999999</v>
+      </c>
+      <c r="AC13" s="9">
+        <v>0.1961</v>
+      </c>
+      <c r="AD13" s="9">
+        <v>0.30030000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.1321</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.75949999999999995</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.34239999999999998</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0.1321</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0.75949999999999995</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0.34239999999999998</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O14" s="9">
+        <v>0.1605</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>0.25290000000000001</v>
+      </c>
+      <c r="R14" s="9">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="T14" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="U14" s="9">
+        <v>0.17910000000000001</v>
+      </c>
+      <c r="V14" s="9">
+        <v>0.63349999999999995</v>
+      </c>
+      <c r="W14" s="9">
+        <v>0.21060000000000001</v>
+      </c>
+      <c r="X14" s="9">
+        <v>0.31619999999999998</v>
+      </c>
+      <c r="Y14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z14" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="AA14" s="9">
+        <v>0.19839999999999999</v>
+      </c>
+      <c r="AB14" s="9">
+        <v>0.59360000000000002</v>
+      </c>
+      <c r="AC14" s="9">
+        <v>0.1782</v>
+      </c>
+      <c r="AD14" s="9">
+        <v>0.27410000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.13189999999999999</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.7389</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.31240000000000001</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0.43909999999999999</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0.13189999999999999</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.7389</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0.31240000000000001</v>
+      </c>
+      <c r="L15" s="9">
+        <v>0.43909999999999999</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O15" s="9">
+        <v>0.15989999999999999</v>
+      </c>
+      <c r="P15" s="9">
+        <v>0.66320000000000001</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>0.23130000000000001</v>
+      </c>
+      <c r="R15" s="9">
+        <v>0.34289999999999998</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T15" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U15" s="9">
+        <v>0.15989999999999999</v>
+      </c>
+      <c r="V15" s="9">
+        <v>0.66320000000000001</v>
+      </c>
+      <c r="W15" s="9">
+        <v>0.23130000000000001</v>
+      </c>
+      <c r="X15" s="9">
+        <v>0.34289999999999998</v>
+      </c>
+      <c r="Y15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>0.1787</v>
+      </c>
+      <c r="AB15" s="9">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>0.19220000000000001</v>
+      </c>
+      <c r="AD15" s="9">
+        <v>0.29289999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.1158</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.84989999999999999</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.37759999999999999</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.52290000000000003</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0.1313</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.7319</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0.28660000000000002</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0.41189999999999999</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O16" s="9">
+        <v>0.1313</v>
+      </c>
+      <c r="P16" s="9">
+        <v>0.7319</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>0.28660000000000002</v>
+      </c>
+      <c r="R16" s="9">
+        <v>0.41189999999999999</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T16" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U16" s="9">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="V16" s="9">
+        <v>0.65469999999999995</v>
+      </c>
+      <c r="W16" s="9">
+        <v>0.2122</v>
+      </c>
+      <c r="X16" s="9">
+        <v>0.32050000000000001</v>
+      </c>
+      <c r="Y16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z16" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="AA16" s="9">
+        <v>0.17730000000000001</v>
+      </c>
+      <c r="AB16" s="9">
+        <v>0.60760000000000003</v>
+      </c>
+      <c r="AC16" s="9">
+        <v>0.17630000000000001</v>
+      </c>
+      <c r="AD16" s="9">
+        <v>0.27329999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.1149</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.84940000000000004</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0.49370000000000003</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0.1149</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0.84940000000000004</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0.49370000000000003</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O17" s="9">
+        <v>0.13059999999999999</v>
+      </c>
+      <c r="P17" s="9">
+        <v>0.73140000000000005</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>0.26350000000000001</v>
+      </c>
+      <c r="R17" s="9">
+        <v>0.38740000000000002</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U17" s="9">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="V17" s="9">
+        <v>0.65439999999999998</v>
+      </c>
+      <c r="W17" s="9">
+        <v>0.1953</v>
+      </c>
+      <c r="X17" s="9">
+        <v>0.30080000000000001</v>
+      </c>
+      <c r="Y17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA17" s="9">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="AB17" s="9">
+        <v>0.65439999999999998</v>
+      </c>
+      <c r="AC17" s="9">
+        <v>0.1953</v>
+      </c>
+      <c r="AD17" s="9">
+        <v>0.30080000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.1144</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.32169999999999999</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0.1144</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.32169999999999999</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0.13009999999999999</v>
+      </c>
+      <c r="P18" s="9">
+        <v>0.73109999999999997</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>0.24349999999999999</v>
+      </c>
+      <c r="R18" s="9">
+        <v>0.36530000000000001</v>
+      </c>
+      <c r="S18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U18" s="9">
+        <v>0.13009999999999999</v>
+      </c>
+      <c r="V18" s="9">
+        <v>0.73109999999999997</v>
+      </c>
+      <c r="W18" s="9">
+        <v>0.24349999999999999</v>
+      </c>
+      <c r="X18" s="9">
+        <v>0.36530000000000001</v>
+      </c>
+      <c r="Y18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z18" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA18" s="9">
+        <v>0.15709999999999999</v>
+      </c>
+      <c r="AB18" s="9">
+        <v>0.65410000000000001</v>
+      </c>
+      <c r="AC18" s="9">
+        <v>0.18049999999999999</v>
+      </c>
+      <c r="AD18" s="9">
+        <v>0.28289999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.13719999999999999</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.78169999999999995</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.31979999999999997</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.45390000000000003</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.13719999999999999</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.78169999999999995</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0.31979999999999997</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0.45390000000000003</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O19" s="9">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="P19" s="9">
+        <v>0.6472</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>0.23860000000000001</v>
+      </c>
+      <c r="R19" s="9">
+        <v>0.34870000000000001</v>
+      </c>
+      <c r="S19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="T19" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U19" s="9">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="V19" s="9">
+        <v>0.6472</v>
+      </c>
+      <c r="W19" s="9">
+        <v>0.23860000000000001</v>
+      </c>
+      <c r="X19" s="9">
+        <v>0.34870000000000001</v>
+      </c>
+      <c r="Y19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z19" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA19" s="9">
+        <v>0.18210000000000001</v>
+      </c>
+      <c r="AB19" s="9">
+        <v>0.57589999999999997</v>
+      </c>
+      <c r="AC19" s="9">
+        <v>0.17760000000000001</v>
+      </c>
+      <c r="AD19" s="9">
+        <v>0.27139999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.16739999999999999</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.78959999999999997</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.33939999999999998</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.47470000000000001</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0.16739999999999999</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.78959999999999997</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0.33939999999999998</v>
+      </c>
+      <c r="L20" s="9">
+        <v>0.47470000000000001</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O20" s="9">
+        <v>0.1867</v>
+      </c>
+      <c r="P20" s="9">
+        <v>0.68240000000000001</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>0.2631</v>
+      </c>
+      <c r="R20" s="9">
+        <v>0.37980000000000003</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="T20" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U20" s="9">
+        <v>0.21970000000000001</v>
+      </c>
+      <c r="V20" s="9">
+        <v>0.61819999999999997</v>
+      </c>
+      <c r="W20" s="9">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="X20" s="9">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="Y20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z20" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="AA20" s="9">
+        <v>0.2359</v>
+      </c>
+      <c r="AB20" s="9">
+        <v>0.54949999999999999</v>
+      </c>
+      <c r="AC20" s="9">
+        <v>0.16769999999999999</v>
+      </c>
+      <c r="AD20" s="9">
+        <v>0.25690000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.79049999999999998</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.35680000000000001</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.49170000000000003</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.1638</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.68330000000000002</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0.27389999999999998</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N21" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O21" s="9">
+        <v>0.1638</v>
+      </c>
+      <c r="P21" s="9">
+        <v>0.68330000000000002</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>0.27389999999999998</v>
+      </c>
+      <c r="R21" s="9">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="S21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T21" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U21" s="9">
+        <v>0.1898</v>
+      </c>
+      <c r="V21" s="9">
+        <v>0.61880000000000002</v>
+      </c>
+      <c r="W21" s="9">
+        <v>0.21410000000000001</v>
+      </c>
+      <c r="X21" s="9">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="Y21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z21" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="AA21" s="9">
+        <v>0.215</v>
+      </c>
+      <c r="AB21" s="9">
+        <v>0.54990000000000006</v>
+      </c>
+      <c r="AC21" s="9">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AD21" s="9">
+        <v>0.25729999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.1447</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.74870000000000003</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.47049999999999997</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0.1447</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0.74870000000000003</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0.47049999999999997</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N22" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O22" s="9">
+        <v>0.1641</v>
+      </c>
+      <c r="P22" s="9">
+        <v>0.64849999999999997</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>0.26190000000000002</v>
+      </c>
+      <c r="R22" s="9">
+        <v>0.37309999999999999</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T22" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U22" s="9">
+        <v>0.18870000000000001</v>
+      </c>
+      <c r="V22" s="9">
+        <v>0.58720000000000006</v>
+      </c>
+      <c r="W22" s="9">
+        <v>0.20619999999999999</v>
+      </c>
+      <c r="X22" s="9">
+        <v>0.30530000000000002</v>
+      </c>
+      <c r="Y22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z22" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="AA22" s="9">
+        <v>0.21329999999999999</v>
+      </c>
+      <c r="AB22" s="9">
+        <v>0.52029999999999998</v>
+      </c>
+      <c r="AC22" s="9">
+        <v>0.16170000000000001</v>
+      </c>
+      <c r="AD22" s="9">
+        <v>0.2467</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.14149999999999999</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.3306</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0.4572</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0.14149999999999999</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0.3306</v>
+      </c>
+      <c r="L23" s="9">
+        <v>0.4572</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O23" s="9">
+        <v>0.16070000000000001</v>
+      </c>
+      <c r="P23" s="9">
+        <v>0.64229999999999998</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>0.25240000000000001</v>
+      </c>
+      <c r="R23" s="9">
+        <v>0.36230000000000001</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T23" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U23" s="9">
+        <v>0.18509999999999999</v>
+      </c>
+      <c r="V23" s="9">
+        <v>0.58130000000000004</v>
+      </c>
+      <c r="W23" s="9">
+        <v>0.1983</v>
+      </c>
+      <c r="X23" s="9">
+        <v>0.29580000000000001</v>
+      </c>
+      <c r="Y23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z23" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA23" s="9">
+        <v>0.18509999999999999</v>
+      </c>
+      <c r="AB23" s="9">
+        <v>0.58130000000000004</v>
+      </c>
+      <c r="AC23" s="9">
+        <v>0.1983</v>
+      </c>
+      <c r="AD23" s="9">
+        <v>0.29580000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.1492</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0.71519999999999995</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.32150000000000001</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0.44359999999999999</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0.1492</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0.71519999999999995</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0.32150000000000001</v>
+      </c>
+      <c r="L24" s="9">
+        <v>0.44359999999999999</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O24" s="9">
+        <v>0.16930000000000001</v>
+      </c>
+      <c r="P24" s="9">
+        <v>0.61990000000000001</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>0.24560000000000001</v>
+      </c>
+      <c r="R24" s="9">
+        <v>0.3518</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U24" s="9">
+        <v>0.16930000000000001</v>
+      </c>
+      <c r="V24" s="9">
+        <v>0.61990000000000001</v>
+      </c>
+      <c r="W24" s="9">
+        <v>0.24560000000000001</v>
+      </c>
+      <c r="X24" s="9">
+        <v>0.3518</v>
+      </c>
+      <c r="Y24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z24" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AB24" s="9">
+        <v>0.5635</v>
+      </c>
+      <c r="AC24" s="9">
+        <v>0.1948</v>
+      </c>
+      <c r="AD24" s="9">
+        <v>0.28960000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.1457</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.72209999999999996</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.3221</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0.1457</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0.72209999999999996</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0.3221</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N25" s="9">
+        <v>0.18</v>
+      </c>
+      <c r="O25" s="9">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="P25" s="9">
+        <v>0.50129999999999997</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>0.2767</v>
+      </c>
+      <c r="R25" s="9">
+        <v>0.35659999999999997</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="T25" s="9">
+        <v>0.18</v>
+      </c>
+      <c r="U25" s="9">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="V25" s="9">
+        <v>0.50129999999999997</v>
+      </c>
+      <c r="W25" s="9">
+        <v>0.2767</v>
+      </c>
+      <c r="X25" s="9">
+        <v>0.35659999999999997</v>
+      </c>
+      <c r="Y25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA25" s="9">
+        <v>0.1875</v>
+      </c>
+      <c r="AB25" s="9">
+        <v>0.57430000000000003</v>
+      </c>
+      <c r="AC25" s="9">
+        <v>0.1991</v>
+      </c>
+      <c r="AD25" s="9">
+        <v>0.29570000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.15079999999999999</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.70630000000000004</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0.31659999999999999</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0.15079999999999999</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0.70630000000000004</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0.31659999999999999</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O26" s="9">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="P26" s="9">
+        <v>0.60780000000000001</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>0.24349999999999999</v>
+      </c>
+      <c r="R26" s="9">
+        <v>0.34770000000000001</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="T26" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U26" s="9">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="V26" s="9">
+        <v>0.60780000000000001</v>
+      </c>
+      <c r="W26" s="9">
+        <v>0.24349999999999999</v>
+      </c>
+      <c r="X26" s="9">
+        <v>0.34770000000000001</v>
+      </c>
+      <c r="Y26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z26" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA26" s="9">
+        <v>0.19220000000000001</v>
+      </c>
+      <c r="AB26" s="9">
+        <v>0.55410000000000004</v>
+      </c>
+      <c r="AC26" s="9">
+        <v>0.19489999999999999</v>
+      </c>
+      <c r="AD26" s="9">
+        <v>0.28839999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.1439</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.31190000000000001</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0.43269999999999997</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0.1439</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0.31190000000000001</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0.43269999999999997</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N27" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O27" s="9">
+        <v>0.1608</v>
+      </c>
+      <c r="P27" s="9">
+        <v>0.6079</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>0.2402</v>
+      </c>
+      <c r="R27" s="9">
+        <v>0.34429999999999999</v>
+      </c>
+      <c r="S27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="T27" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U27" s="9">
+        <v>0.1608</v>
+      </c>
+      <c r="V27" s="9">
+        <v>0.6079</v>
+      </c>
+      <c r="W27" s="9">
+        <v>0.2402</v>
+      </c>
+      <c r="X27" s="9">
+        <v>0.34429999999999999</v>
+      </c>
+      <c r="Y27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z27" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA27" s="9">
+        <v>0.18290000000000001</v>
+      </c>
+      <c r="AB27" s="9">
+        <v>0.55420000000000003</v>
+      </c>
+      <c r="AC27" s="9">
+        <v>0.1925</v>
+      </c>
+      <c r="AD27" s="9">
+        <v>0.28570000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.14510000000000001</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.66649999999999998</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.31359999999999999</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0.42649999999999999</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0.14510000000000001</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0.66649999999999998</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0.31359999999999999</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0.42649999999999999</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N28" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O28" s="9">
+        <v>0.15909999999999999</v>
+      </c>
+      <c r="P28" s="9">
+        <v>0.5504</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>0.23630000000000001</v>
+      </c>
+      <c r="R28" s="9">
+        <v>0.3306</v>
+      </c>
+      <c r="S28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="T28" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U28" s="9">
+        <v>0.15909999999999999</v>
+      </c>
+      <c r="V28" s="9">
+        <v>0.5504</v>
+      </c>
+      <c r="W28" s="9">
+        <v>0.23630000000000001</v>
+      </c>
+      <c r="X28" s="9">
+        <v>0.3306</v>
+      </c>
+      <c r="Y28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z28" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="AA28" s="9">
+        <v>0.19839999999999999</v>
+      </c>
+      <c r="AB28" s="9">
+        <v>0.59360000000000002</v>
+      </c>
+      <c r="AC28" s="9">
+        <v>0.1782</v>
+      </c>
+      <c r="AD28" s="9">
+        <v>0.27410000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.67290000000000005</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0.4355</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0.67290000000000005</v>
+      </c>
+      <c r="K29" s="9">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="L29" s="9">
+        <v>0.4355</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0.16569999999999999</v>
+      </c>
+      <c r="P29" s="9">
+        <v>0.55389999999999995</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>0.2389</v>
+      </c>
+      <c r="R29" s="9">
+        <v>0.33379999999999999</v>
+      </c>
+      <c r="S29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="T29" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U29" s="9">
+        <v>0.16569999999999999</v>
+      </c>
+      <c r="V29" s="9">
+        <v>0.55389999999999995</v>
+      </c>
+      <c r="W29" s="9">
+        <v>0.2389</v>
+      </c>
+      <c r="X29" s="9">
+        <v>0.33379999999999999</v>
+      </c>
+      <c r="Y29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z29" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA29" s="9">
+        <v>0.18820000000000001</v>
+      </c>
+      <c r="AB29" s="9">
+        <v>0.49930000000000002</v>
+      </c>
+      <c r="AC29" s="9">
+        <v>0.18959999999999999</v>
+      </c>
+      <c r="AD29" s="9">
+        <v>0.27489999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0.1434</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0.67879999999999996</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0.32790000000000002</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0.44219999999999998</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I30" s="9">
+        <v>0.1434</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0.67879999999999996</v>
+      </c>
+      <c r="K30" s="9">
+        <v>0.32790000000000002</v>
+      </c>
+      <c r="L30" s="9">
+        <v>0.44219999999999998</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N30" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O30" s="9">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="P30" s="9">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>0.2404</v>
+      </c>
+      <c r="R30" s="9">
+        <v>0.3362</v>
+      </c>
+      <c r="S30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="T30" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U30" s="9">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="V30" s="9">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="W30" s="9">
+        <v>0.2404</v>
+      </c>
+      <c r="X30" s="9">
+        <v>0.3362</v>
+      </c>
+      <c r="Y30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z30" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA30" s="9">
+        <v>0.18590000000000001</v>
+      </c>
+      <c r="AB30" s="9">
+        <v>0.50470000000000004</v>
+      </c>
+      <c r="AC30" s="9">
+        <v>0.188</v>
+      </c>
+      <c r="AD30" s="9">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.68479999999999996</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0.3362</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I31" s="9">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0.68479999999999996</v>
+      </c>
+      <c r="K31" s="9">
+        <v>0.3362</v>
+      </c>
+      <c r="L31" s="9">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N31" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O31" s="9">
+        <v>0.1676</v>
+      </c>
+      <c r="P31" s="9">
+        <v>0.56069999999999998</v>
+      </c>
+      <c r="Q31" s="9">
+        <v>0.24310000000000001</v>
+      </c>
+      <c r="R31" s="9">
+        <v>0.3392</v>
+      </c>
+      <c r="S31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="T31" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U31" s="9">
+        <v>0.1676</v>
+      </c>
+      <c r="V31" s="9">
+        <v>0.56069999999999998</v>
+      </c>
+      <c r="W31" s="9">
+        <v>0.24310000000000001</v>
+      </c>
+      <c r="X31" s="9">
+        <v>0.3392</v>
+      </c>
+      <c r="Y31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z31" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA31" s="9">
+        <v>0.19339999999999999</v>
+      </c>
+      <c r="AB31" s="9">
+        <v>0.49980000000000002</v>
+      </c>
+      <c r="AC31" s="9">
+        <v>0.18770000000000001</v>
+      </c>
+      <c r="AD31" s="9">
+        <v>0.27289999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.14269999999999999</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.69350000000000001</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0.34639999999999999</v>
+      </c>
+      <c r="F32" s="9">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I32" s="9">
+        <v>0.14269999999999999</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.69350000000000001</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0.34639999999999999</v>
+      </c>
+      <c r="L32" s="9">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N32" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O32" s="9">
+        <v>0.16259999999999999</v>
+      </c>
+      <c r="P32" s="9">
+        <v>0.56950000000000001</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>0.24959999999999999</v>
+      </c>
+      <c r="R32" s="9">
+        <v>0.34710000000000002</v>
+      </c>
+      <c r="S32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T32" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U32" s="9">
+        <v>0.16259999999999999</v>
+      </c>
+      <c r="V32" s="9">
+        <v>0.56950000000000001</v>
+      </c>
+      <c r="W32" s="9">
+        <v>0.24959999999999999</v>
+      </c>
+      <c r="X32" s="9">
+        <v>0.34710000000000002</v>
+      </c>
+      <c r="Y32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z32" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA32" s="9">
+        <v>0.18920000000000001</v>
+      </c>
+      <c r="AB32" s="9">
+        <v>0.50160000000000005</v>
+      </c>
+      <c r="AC32" s="9">
+        <v>0.189</v>
+      </c>
+      <c r="AD32" s="9">
+        <v>0.27450000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0.1358</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.69350000000000001</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0.1358</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.69350000000000001</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="M33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N33" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="O33" s="9">
+        <v>0.1545</v>
+      </c>
+      <c r="P33" s="9">
+        <v>0.56950000000000001</v>
+      </c>
+      <c r="Q33" s="9">
+        <v>0.2492</v>
+      </c>
+      <c r="R33" s="9">
+        <v>0.34670000000000001</v>
+      </c>
+      <c r="S33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T33" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U33" s="9">
+        <v>0.1545</v>
+      </c>
+      <c r="V33" s="9">
+        <v>0.56950000000000001</v>
+      </c>
+      <c r="W33" s="9">
+        <v>0.2492</v>
+      </c>
+      <c r="X33" s="9">
+        <v>0.34670000000000001</v>
+      </c>
+      <c r="Y33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z33" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA33" s="9">
+        <v>0.18210000000000001</v>
+      </c>
+      <c r="AB33" s="9">
+        <v>0.57589999999999997</v>
+      </c>
+      <c r="AC33" s="9">
+        <v>0.17760000000000001</v>
+      </c>
+      <c r="AD33" s="9">
+        <v>0.27139999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="S1:X1"/>
+    <mergeCell ref="Y1:AD1"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>